<commit_message>
Data documentation file added
</commit_message>
<xml_diff>
--- a/data_documentation/data_documentation.xlsx
+++ b/data_documentation/data_documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://brown365-my.sharepoint.com/personal/flu14_ad_brown_edu/Documents/Desktop/RA/LinkagePaper/FileDocumentation/GitUpload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{7D455F3C-7EE1-401E-98B4-EA4AF3E1ADD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF3A2EF1-19FB-480E-AE97-407AEA2826F8}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{7D455F3C-7EE1-401E-98B4-EA4AF3E1ADD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF786739-CD9B-414A-B58C-0FEBDA133878}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{19A07E2F-66D0-4231-B040-A3BFA5B642FD}"/>
   </bookViews>
@@ -470,6 +470,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -935,11 +939,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DCBBF3-534E-45ED-8D4A-1E351893D2BA}">
-  <dimension ref="A2:D36"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -950,40 +954,54 @@
     <col min="4" max="4" width="51.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="A2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -991,13 +1009,13 @@
         <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -1005,13 +1023,13 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -1019,13 +1037,13 @@
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -1033,13 +1051,13 @@
         <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -1047,27 +1065,27 @@
         <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -1075,13 +1093,13 @@
         <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -1089,13 +1107,13 @@
         <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -1103,27 +1121,27 @@
         <v>24</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -1131,13 +1149,13 @@
         <v>25</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -1145,13 +1163,13 @@
         <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -1159,13 +1177,13 @@
         <v>25</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -1173,13 +1191,13 @@
         <v>25</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -1187,13 +1205,13 @@
         <v>25</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -1201,13 +1219,13 @@
         <v>25</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -1215,13 +1233,13 @@
         <v>25</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -1229,13 +1247,13 @@
         <v>25</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -1243,13 +1261,13 @@
         <v>25</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -1257,13 +1275,13 @@
         <v>25</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -1271,49 +1289,49 @@
         <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="A26" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="15"/>
+      <c r="A27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -1321,27 +1339,27 @@
         <v>22</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -1349,27 +1367,27 @@
         <v>66</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -1377,59 +1395,45 @@
         <v>23</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="A34" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="15"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="15"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
+      <c r="A35" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B16:B26">
-    <sortCondition ref="B16:B26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B15:B25">
+    <sortCondition ref="B15:B25"/>
   </sortState>
   <mergeCells count="3">
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A34:D34"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>